<commit_message>
Mainly changed building placement (details in desc)
The buildable base and vehicle pad are now actual buildings. Buildings
are placed similiar to dragging stuff (same system as BECTI)

Mission now uses R3F instead of BTC logistics

Fatigue seems to be disabled now
</commit_message>
<xml_diff>
--- a/Documentation/todo_history.xlsx
+++ b/Documentation/todo_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -37,14 +37,32 @@
     <t>Enemy Spawning in Cities must be more dependent on the players progress  and on the number of players</t>
   </si>
   <si>
-    <t>Somehow mark the bases and vehicle refit station, maybe take a look at the building placement from BECTI</t>
+    <t>Completely disable fatigue. The players have to run to much to have it enabled.</t>
+  </si>
+  <si>
+    <t>Somehow mark the bases and vehicle refit station (not just on the map), maybe take a look at the building placement from BECTI</t>
+  </si>
+  <si>
+    <t>First respawn is sometimes set on grid 000000</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>11.30</t>
+  </si>
+  <si>
+    <t>Some Objects can not be dragged / loaded</t>
+  </si>
+  <si>
+    <t>Dead Enemies lose their gear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +74,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -90,6 +122,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -394,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,36 +475,80 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>41885</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="7">
+        <v>41885</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>41885</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="4">
+        <v>41885</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>41885</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="4">
+        <v>41885</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>41885</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>41885</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>41885</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>41885</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dead men tell no tales
Enemies now lose their gear upon death
</commit_message>
<xml_diff>
--- a/Documentation/todo_history.xlsx
+++ b/Documentation/todo_history.xlsx
@@ -55,14 +55,14 @@
     <t>Some Objects can not be dragged / loaded</t>
   </si>
   <si>
-    <t>Dead Enemies lose their gear</t>
+    <t>Dead Enemies should lose their gear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +80,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -87,7 +94,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF92D050"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,6 +143,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -443,7 +457,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="A5:C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,35 +489,35 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>41885</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="10">
+        <v>41885</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>41885</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="7">
+        <v>41885</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>41885</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="7">
+        <v>41885</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -519,13 +533,13 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>41885</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="10">
+        <v>41885</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -541,13 +555,13 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>41885</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="7">
+        <v>41885</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Player start with map & changed enemy spawning
More Players = more spawning!
</commit_message>
<xml_diff>
--- a/Documentation/todo_history.xlsx
+++ b/Documentation/todo_history.xlsx
@@ -62,7 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,13 +92,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,14 +113,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -143,13 +130,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -456,9 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -467,101 +445,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>41885</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2">
+        <v>41885</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>41885</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="5">
+        <v>41885</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>41885</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="5">
+        <v>41885</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>41885</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="5">
+        <v>41885</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>41885</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="5">
+        <v>41885</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>41885</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="5">
+        <v>41885</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>41885</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="2">
+        <v>41885</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>41885</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="5">
+        <v>41885</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I have a dream. Of change.
- ais-injury but has a bug that the 3d icon isnt remove sometimes
- Experienced an ais-injury script error once (observate)
- NAMETAGS! Every object can be have an individual nametag assigned to
it
- Lootspawner variables changed, more backpacks and attachments
</commit_message>
<xml_diff>
--- a/Documentation/todo_history.xlsx
+++ b/Documentation/todo_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -59,13 +59,28 @@
   </si>
   <si>
     <t>Enemy skill customizable</t>
+  </si>
+  <si>
+    <t>13.10</t>
+  </si>
+  <si>
+    <t>More backbacks dropped in houses or guaranteed backpack in "Wildness" / "Houses" type as loot</t>
+  </si>
+  <si>
+    <t>Loot Vehicles should have empty cargo</t>
+  </si>
+  <si>
+    <t>Disable red markers in occupied houses</t>
+  </si>
+  <si>
+    <t>More scopes dropped</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +110,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -116,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -139,6 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -443,17 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="161" customWidth="1"/>
+    <col min="3" max="3" width="161" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -534,13 +554,13 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>41885</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="5">
+        <v>41885</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -564,6 +584,50 @@
       </c>
       <c r="C10" s="7" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>41888</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>41888</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>41888</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>41888</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes on target-generating and loot
- Through a logical mistake there were very few units generated at each
target. The number of enemies now doesn't depend on the players progress
anymore. The mission now might be harder in the beginning.

- It was really hard to get 4th and 5th tier weapons and ammo. Better
objects are now easier to obtain (loot changes)

- Advanced start doesn't grant as many objects anymore. Especially there
are fewer vehicles.

- Some changes for lifting in the logistics system. Whole thing needs to
be rethought.

- Changed the description and added and overview/loading picture
</commit_message>
<xml_diff>
--- a/Documentation/todo_history.xlsx
+++ b/Documentation/todo_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -100,14 +100,35 @@
     <t>Apparently "Anthrakia" is registered as a big city</t>
   </si>
   <si>
-    <t>Big Cities have 4 tanks from the beginning, and that with 2 players !!!!!-----&gt; KI was activated, thus 6 players were handled</t>
+    <t>18.40</t>
+  </si>
+  <si>
+    <t>Recheck the R3F-Config-Lists in plugins\R3F_LOG\addons_config\A3_vanilla_1.22</t>
+  </si>
+  <si>
+    <t>Recode the number of patrols, for each target</t>
+  </si>
+  <si>
+    <t>Some ammoboxes exploded, they seem to take damage, when manually setting allowdamage to false (by console) the don't take damage anymore</t>
+  </si>
+  <si>
+    <t>Communication options disappear when a save mission is loaded</t>
+  </si>
+  <si>
+    <t>21.00</t>
+  </si>
+  <si>
+    <t>Logical mistake when determining the amount of enemies per target, the whole determination has been changed now</t>
+  </si>
+  <si>
+    <t>Recoded the amount of loot, god tier weapons were almost impossible to get</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +164,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -191,6 +220,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -495,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,25 +754,80 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="11">
         <v>41894</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>28</v>
+      <c r="C20" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
-        <v>41894</v>
+        <v>41956</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>41956</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>41956</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>41956</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>41957</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>41957</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logistic properties done correctly
</commit_message>
<xml_diff>
--- a/Documentation/todo_history.xlsx
+++ b/Documentation/todo_history.xlsx
@@ -534,7 +534,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C21" sqref="A21:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,13 +765,13 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="5">
         <v>41956</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="7" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Communication menu on dedicated
</commit_message>
<xml_diff>
--- a/Documentation/todo_history.xlsx
+++ b/Documentation/todo_history.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Todo &amp; History" sheetId="1" r:id="rId1"/>
+    <sheet name="Suggestions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +124,51 @@
   <si>
     <t>Some ammoboxes exploded, they seem to take damage, when manually setting allowdamage to false (by console) the don't take damage anymore
 Update 15.11/10.30: When dragging or loading an ammobox, it seems like a new one is created which allows damage</t>
+  </si>
+  <si>
+    <t>20.45</t>
+  </si>
+  <si>
+    <t>On Dedicated, communication menus didn't appear, needs new testing</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>Zombie Module</t>
+  </si>
+  <si>
+    <t>There exists a zombie mission, at the moment abandoned, which doesn't require a mod to spawn (low quality) zombies. Zombies could just spawn around houses or around the player and be an extra threat.</t>
+  </si>
+  <si>
+    <t>Patrolling Enemies</t>
+  </si>
+  <si>
+    <t>Was planed but never implemented. Units can be created at random which will patrol from one target to another. Important is that they don't patrol around conquered targets, so that the players are safe around them. We might make an option to disable AT and AA soldiers, so it's still somewhat safe to drive around.</t>
+  </si>
+  <si>
+    <t>Apocalypse Module</t>
+  </si>
+  <si>
+    <t>I heard about a mod which adds apocalyptic stuff to Arma. Apparently there are catastrophes like tornados or earthquakes, which could be another threat.</t>
+  </si>
+  <si>
+    <t>More Advanced Start Options</t>
+  </si>
+  <si>
+    <t>Additional to the existing advanced start, there should be more options. For example that one assault rifle or launcher is granted or just a vehicle without equipment.</t>
+  </si>
+  <si>
+    <t>Mod Content as Modules</t>
+  </si>
+  <si>
+    <t>For more variety and customization to the mission, the host should be able to act- resp. deactivate content as modules. For each module should exist a parameter.</t>
+  </si>
+  <si>
+    <t>Mod Content (like Weapons and Vehicles) can also be activated by parameters. There should be a parameter for each mod.</t>
   </si>
 </sst>
 </file>
@@ -194,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -233,6 +279,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="A22:C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,8 +895,161 @@
         <v>34</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>41965</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="190.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="20"/>
+    </row>
+    <row r="9" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="20"/>
+    </row>
+    <row r="10" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="20"/>
+    </row>
+    <row r="11" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="20"/>
+    </row>
+    <row r="12" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="20"/>
+    </row>
+    <row r="13" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="20"/>
+    </row>
+    <row r="14" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="20"/>
+    </row>
+    <row r="15" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="20"/>
+    </row>
+    <row r="16" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="20"/>
+    </row>
+    <row r="17" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="20"/>
+    </row>
+    <row r="18" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="20"/>
+    </row>
+    <row r="19" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="20"/>
+    </row>
+    <row r="20" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="20"/>
+    </row>
+    <row r="21" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+    </row>
+    <row r="22" spans="1:2" s="19" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" s="19" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Helicopter and comm. menu fix
- Helicopters are too much of a threat when driving around, they now
only spawn at airports

- Communication Menu entries should now appear on dedicated servers

- Fixed a naming bug for nametags
</commit_message>
<xml_diff>
--- a/Documentation/todo_history.xlsx
+++ b/Documentation/todo_history.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Todo &amp; History" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>10.30</t>
-  </si>
-  <si>
-    <t>Players sometimes stay on the spawn island resp. aren't teleported</t>
   </si>
   <si>
     <t>Some ammoboxes exploded, they seem to take damage, when manually setting allowdamage to false (by console) the don't take damage anymore
@@ -169,6 +166,18 @@
   </si>
   <si>
     <t>Mod Content (like Weapons and Vehicles) can also be activated by parameters. There should be a parameter for each mod.</t>
+  </si>
+  <si>
+    <t>Players sometimes stay on the spawn island resp. aren't teleported or are on position 000000 (ocean)</t>
+  </si>
+  <si>
+    <t>15.45</t>
+  </si>
+  <si>
+    <t>Sometimes weapons disappear when being revived</t>
+  </si>
+  <si>
+    <t>Helicopters are too big of a threat, they should only appear around airfields</t>
   </si>
 </sst>
 </file>
@@ -240,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -291,6 +300,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="A29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +869,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,18 +913,40 @@
         <v>33</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+      <c r="A27" s="21">
         <v>41965</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>37</v>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>41967</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="23">
+        <v>41967</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -916,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -926,7 +969,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -934,50 +977,50 @@
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>44</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>46</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Parameter for dedicated changed
</commit_message>
<xml_diff>
--- a/Documentation/todo_history.xlsx
+++ b/Documentation/todo_history.xlsx
@@ -104,9 +104,6 @@
     <t>Recode the number of patrols, for each target</t>
   </si>
   <si>
-    <t>Communication options disappear when a save mission is loaded</t>
-  </si>
-  <si>
     <t>21.00</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Helicopters are too big of a threat, they should only appear around airfields</t>
+  </si>
+  <si>
+    <t>Communication options disappear when a save mission is loaded. However when adding just 1 entry, all of them appear again</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="A29:C29"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,7 +869,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,10 +888,10 @@
         <v>41957</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,10 +899,10 @@
         <v>41957</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,10 +910,10 @@
         <v>41958</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -921,10 +921,10 @@
         <v>41965</v>
       </c>
       <c r="B27" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,10 +932,10 @@
         <v>41967</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,10 +943,10 @@
         <v>41967</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -969,7 +969,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -977,50 +977,50 @@
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>